<commit_message>
Make WorkerLimit editable from Config.xlsx
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\UiPath\ReFrameWork\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\AppData\Local\UiPath\ProjectTemplates\Parallel Background RE Framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCF8DB8-7FC9-4431-9470-1ACA5C8F70AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D093879-76C1-41AF-8528-49C70B5C31C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>This is an example how to use this sheet. 'Name' is the name in the Credential Dictionary inside the Framework. Credential Name is the name which will be requested from user or orchestrator via invoke GetAppCredentials.</t>
+  </si>
+  <si>
+    <t>BusinessProcess_ParallelExecutions</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -554,29 +559,29 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1579,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212F9408-6F55-4141-8442-906F0AC16FC0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2674,8 +2679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2801,7 +2806,14 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Log Messages on a seperate sheet. Remove Application logic, because its a background-proccessing framework. Added missing reference arguments (ProcessReference and WorkerReferences)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\AppData\Local\UiPath\ProjectTemplates\Parallel Background RE Framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E22C9D-9D69-4210-A019-A586D4DA101E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05209231-F683-4D38-8AE8-5BB46C27E5BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="10875" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6405" yWindow="4140" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Credentials" sheetId="4" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
     <sheet name="Constants" sheetId="2" r:id="rId4"/>
+    <sheet name="Messages" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -40,15 +41,6 @@
     <t>Description (Assets will always overwrite other config)</t>
   </si>
   <si>
-    <t>MaxRetryNumber</t>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
     <t>Exceptions_Screenshots</t>
   </si>
   <si>
@@ -58,34 +50,16 @@
     <t>LogMessage_GetTransactionData</t>
   </si>
   <si>
-    <t>Static part of logging message. Calling Get Transaction Data</t>
-  </si>
-  <si>
     <t>LogMessage_GetTransactionDataError</t>
   </si>
   <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
     <t>LogMessage_Success</t>
   </si>
   <si>
-    <t>Static part of logging message. Processed Transaction succesful</t>
-  </si>
-  <si>
     <t>LogMessage_BusinessRuleException</t>
   </si>
   <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception</t>
-  </si>
-  <si>
     <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
@@ -134,6 +108,48 @@
   </si>
   <si>
     <t>Business rule exception in worker '{0}'. Reason: {1}.</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>If this is true the framework will use an Orchestrator Queue to retrieve data. If false. InitTransactiondata will be called and "GetTransactiondataFromDataStructure" will be invoked</t>
+  </si>
+  <si>
+    <t>Framework_OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Framework_UseOrchestratorQueue</t>
+  </si>
+  <si>
+    <t>Framework_MaxRetryNumber</t>
+  </si>
+  <si>
+    <t>Does not have any effect if "UseOrchestratorQueue" is set to true. If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
+  </si>
+  <si>
+    <t>Framework_ExScreenshotsFolderPath</t>
+  </si>
+  <si>
+    <t>LogMessage_DisposingProcessDataException</t>
+  </si>
+  <si>
+    <t>The limit of parallel Workers.</t>
+  </si>
+  <si>
+    <t>Disposing process data failed due to an exception. Reason {0} at activity '{1}'</t>
+  </si>
+  <si>
+    <t>LogMessage_WorkerFinished</t>
+  </si>
+  <si>
+    <t>All worker finished there work</t>
+  </si>
+  <si>
+    <t>Framework_FaultOnAppOrBRException</t>
+  </si>
+  <si>
+    <t>Indicate if the Framework should rethrow the error if a transaction wasnt succesful. "MaxRetryNumber" ist taken into account. Usefull if you use mediarecording for processes.</t>
   </si>
 </sst>
 </file>
@@ -185,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -194,6 +210,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,7 +537,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -559,27 +584,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1598,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1606,13 +1620,13 @@
     </row>
     <row r="2" spans="1:3" ht="60">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2675,10 +2689,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2723,95 +2737,82 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" ht="30">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="30">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+    <row r="8" spans="1:26" ht="30">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3777,18 +3778,118 @@
     <row r="976" ht="14.25" customHeight="1"/>
     <row r="977" ht="14.25" customHeight="1"/>
     <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A4AFB5-D336-4781-BD6F-5D1870C4CE37}">
+  <dimension ref="A1:Z8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added an option to choose if an orchestrator queue will be used or a blockingcollection
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\AppData\Local\UiPath\ProjectTemplates\Parallel Background RE Framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05209231-F683-4D38-8AE8-5BB46C27E5BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F17E15-ED94-48C5-8B9A-C8EFD18F5028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="4140" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22635" yWindow="4290" windowWidth="20910" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>ProcessABCQueue</t>
@@ -146,10 +143,25 @@
     <t>All worker finished there work</t>
   </si>
   <si>
-    <t>Framework_FaultOnAppOrBRException</t>
-  </si>
-  <si>
-    <t>Indicate if the Framework should rethrow the error if a transaction wasnt succesful. "MaxRetryNumber" ist taken into account. Usefull if you use mediarecording for processes.</t>
+    <t>LogMessage_BusinessRuleExceptionDetails</t>
+  </si>
+  <si>
+    <t>LogMessage_ApplicationExceptionDetails</t>
+  </si>
+  <si>
+    <t>Activity {0} has thrown the error.</t>
+  </si>
+  <si>
+    <t>Please review the QueueItem definition and correct the error.</t>
+  </si>
+  <si>
+    <t>LogMessage_WorkerInitialized</t>
+  </si>
+  <si>
+    <t>Worker '{0}' initialized.</t>
+  </si>
+  <si>
+    <t>Parallel Background Framework</t>
   </si>
 </sst>
 </file>
@@ -204,7 +216,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -218,6 +229,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -537,25 +551,25 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43" style="2" customWidth="1"/>
     <col min="3" max="3" width="68.5703125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="18.75">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1"/>
@@ -582,15 +596,15 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" ht="30">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1597,36 +1611,36 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1638,24 +1652,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" style="2" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="18.75">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1"/>
@@ -2691,122 +2707,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41" style="2" customWidth="1"/>
+    <col min="2" max="2" width="87.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="18.75">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>35</v>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="30">
-      <c r="A4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="30">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="30">
-      <c r="A8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>40</v>
-      </c>
+    <row r="8" spans="1:26">
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3786,10 +3792,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A4AFB5-D336-4781-BD6F-5D1870C4CE37}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3799,14 +3805,14 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="18.75">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1"/>
@@ -3834,60 +3840,94 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
-    <row r="8" spans="1:26">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
+    <row r="11" spans="1:26">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rework most of the project descriptions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\AppData\Local\UiPath\ProjectTemplates\Parallel Background RE Framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F17E15-ED94-48C5-8B9A-C8EFD18F5028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49F5728-7982-4DA2-B366-AEF970537BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22635" yWindow="4290" windowWidth="20910" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Processing transaction {0} in worker '{1}'.</t>
   </si>
   <si>
-    <t>Error getting transaction data for Transaction Number {0} in Worker '{1}'. Reason: {2} at Source {3}</t>
-  </si>
-  <si>
-    <t>Worker '{0}' completted a transaction successfully.</t>
-  </si>
-  <si>
     <t>System exception in worker '{0}'. Reason: {1}.</t>
   </si>
   <si>
@@ -134,15 +128,9 @@
     <t>The limit of parallel Workers.</t>
   </si>
   <si>
-    <t>Disposing process data failed due to an exception. Reason {0} at activity '{1}'</t>
-  </si>
-  <si>
     <t>LogMessage_WorkerFinished</t>
   </si>
   <si>
-    <t>All worker finished there work</t>
-  </si>
-  <si>
     <t>LogMessage_BusinessRuleExceptionDetails</t>
   </si>
   <si>
@@ -162,6 +150,51 @@
   </si>
   <si>
     <t>Parallel Background Framework</t>
+  </si>
+  <si>
+    <t>LogMessage_DisposingProcessData</t>
+  </si>
+  <si>
+    <t>Dispose process data ...</t>
+  </si>
+  <si>
+    <t>LogMessage_InitializeProcessData</t>
+  </si>
+  <si>
+    <t>Initialize process data ...</t>
+  </si>
+  <si>
+    <t>LogMessage_StopRequested</t>
+  </si>
+  <si>
+    <t>LogMessage_DisposingWorkerDataException</t>
+  </si>
+  <si>
+    <t>Disposing worker references failed due to an exception. Reason {0} at activity '{1}'</t>
+  </si>
+  <si>
+    <t>Disposing process references failed due to an exception. Reason {0} at activity '{1}'</t>
+  </si>
+  <si>
+    <t>Worker '{0}' completed a transaction successfully.</t>
+  </si>
+  <si>
+    <t>Error getting transaction data for transaction number {0} in Worker '{1}'. Reason: {2} at Source {3}</t>
+  </si>
+  <si>
+    <t>All worker finished there work!</t>
+  </si>
+  <si>
+    <t>Stop requested for Worker {0}.</t>
+  </si>
+  <si>
+    <t>{0] is reserverted for the asset name</t>
+  </si>
+  <si>
+    <t>Loading Credential with internal name {0} failed. Reason: {1}</t>
+  </si>
+  <si>
+    <t>LogMessage_ConfigLoadCredentialFailed</t>
   </si>
 </sst>
 </file>
@@ -601,7 +634,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -2761,7 +2794,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -2769,18 +2802,18 @@
     </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -2791,18 +2824,18 @@
     </row>
     <row r="6" spans="1:26" ht="30">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -3792,10 +3825,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A4AFB5-D336-4781-BD6F-5D1870C4CE37}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3853,7 +3886,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3862,7 +3895,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -3871,16 +3904,16 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -3889,45 +3922,89 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correct "LogMessage_LogMessage" to "LogMessage_"
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\UiPath2\UiPath-Parallel-Background-RE-Framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4D6875-150C-4CF8-9DE5-E7C67902DFC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AEAEF8-B55F-4AF5-A8DE-2B56AEB41410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29280" yWindow="4440" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27450" yWindow="4560" windowWidth="20910" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>Worker {0} finished due to no more transaction data</t>
+  </si>
+  <si>
+    <t>LogMessage_InitializeWorkerdata</t>
+  </si>
+  <si>
+    <t>Initialize data for Worker {0} ...</t>
   </si>
 </sst>
 </file>
@@ -3837,10 +3843,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A4AFB5-D336-4781-BD6F-5D1870C4CE37}">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4034,6 +4040,14 @@
         <v>59</v>
       </c>
     </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>